<commit_message>
Manual Test Case Templates
</commit_message>
<xml_diff>
--- a/Manual Testing Template.xlsx
+++ b/Manual Testing Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7323E5-0198-4A3A-9DE4-33445D0CDDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C0C7B6-487A-4712-AEB2-0129B337AD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{034F2C79-1E6B-4C5D-B245-C697B396B7EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Project Name:</t>
   </si>
@@ -177,6 +177,36 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_003</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter valid password
+3. Click on the Login button</t>
+  </si>
+  <si>
+    <t>Username: xxxx@erp.com
+Password: P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Enter an invalid username &amp; an invalid password</t>
+  </si>
+  <si>
+    <t>Enter an invalid username &amp; a valid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter invalid password
+3. Click on the Login button</t>
+  </si>
+  <si>
+    <t>Username: xxxx@erp.com
+Password: xxxxxxxx</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_004</t>
   </si>
 </sst>
 </file>
@@ -184,7 +214,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="ddd\,/dd/mmm\,/yyyy"/>
+    <numFmt numFmtId="165" formatCode="ddd/dd/mmm\,/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -197,19 +227,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -283,21 +325,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -358,7 +385,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -367,49 +394,19 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -418,9 +415,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -431,79 +426,110 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -513,65 +539,405 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="ddd/dd/mmm\,/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -582,6 +948,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{23CF6551-BF7D-4203-BC4C-7D7432EF6610}" name="Table1" displayName="Table1" ref="A10:N14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16">
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{0CBF9EE2-DD2D-42EA-B633-8B7D9F255B39}" name="Test Scenario ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{C2E0D337-2D3D-4D5E-A84B-34A27362695C}" name="Test Scenario Description" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{606D9537-F85C-4652-B36F-89BE6F233FF6}" name="Test Case ID" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{5DAA1AB1-4998-42D7-A489-8F422706446C}" name="Test Case Description" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{6737D86F-F1AA-42D1-BBF8-36DF94DDCA54}" name="Test Steps" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{59DF8DD1-DBDD-4CE7-8642-C7A036502BC6}" name="Pre-Condition" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{DB15279D-42EB-4E58-816D-230AEF3A371F}" name="Test Data" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{5472CED6-2868-4880-B2A5-B016FAEAEE9F}" name="Post-Condition" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{A543F2A4-ADFB-4993-859B-53802ADED585}" name="Expected Result" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{8DD8B8FB-5241-473E-9BCA-2C2757979A90}" name="Actual Result" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{9CF89F2B-97C2-4B4A-B1A4-CAB4CF52E33B}" name="Status" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{E1876C0F-8407-434B-B306-42CBC2E4AE35}" name="Executed By" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{307707D3-252B-4F10-911E-782B3D99649C}" name="Execution Date" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{16DB1863-C5A5-443F-BF3D-D834543FC628}" name="Comments (If Any)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -881,245 +1269,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028BB32B-4B47-4368-8F5D-9005778AD63A}">
-  <dimension ref="A3:N14"/>
+  <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
     <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="16">
         <v>44741</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="17">
         <v>44755</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:14" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="26" t="s">
+      <c r="M10" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="36" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M11" s="8">
         <v>41091</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="6" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:14" s="4" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="30">
+      <c r="M12" s="9">
         <v>41092</v>
       </c>
       <c r="N12" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="23"/>
+    <row r="13" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="9">
+        <v>41093</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="19"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="24"/>
+    <row r="14" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="29">
+        <v>41094</v>
+      </c>
+      <c r="N14" s="30" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>